<commit_message>
Eggerland - several more rooms done.
</commit_message>
<xml_diff>
--- a/trunk/Eggerland/Eggerland.xlsx
+++ b/trunk/Eggerland/Eggerland.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>Enter room</t>
   </si>
@@ -49,6 +49,24 @@
   </si>
   <si>
     <t>Room begin</t>
+  </si>
+  <si>
+    <t>Destroy egg</t>
+  </si>
+  <si>
+    <t>Square appears</t>
+  </si>
+  <si>
+    <t>Get heart</t>
+  </si>
+  <si>
+    <t>Get Raft</t>
+  </si>
+  <si>
+    <t>Get raft</t>
+  </si>
+  <si>
+    <t>Get Key</t>
   </si>
 </sst>
 </file>
@@ -380,15 +398,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -510,7 +528,7 @@
         <v>44087</v>
       </c>
       <c r="D11">
-        <f>C11-B11</f>
+        <f t="shared" ref="D11:D32" si="0">C11-B11</f>
         <v>-1056</v>
       </c>
     </row>
@@ -525,7 +543,7 @@
         <v>45376</v>
       </c>
       <c r="D12">
-        <f>C12-B12</f>
+        <f t="shared" si="0"/>
         <v>-1057</v>
       </c>
     </row>
@@ -540,7 +558,7 @@
         <v>45734</v>
       </c>
       <c r="D13">
-        <f>C13-B13</f>
+        <f t="shared" si="0"/>
         <v>-1057</v>
       </c>
     </row>
@@ -555,7 +573,7 @@
         <v>47058</v>
       </c>
       <c r="D14">
-        <f>C14-B14</f>
+        <f t="shared" si="0"/>
         <v>-1056</v>
       </c>
     </row>
@@ -570,7 +588,7 @@
         <v>49834</v>
       </c>
       <c r="D15">
-        <f>C15-B15</f>
+        <f t="shared" si="0"/>
         <v>-1055</v>
       </c>
     </row>
@@ -585,7 +603,7 @@
         <v>50428</v>
       </c>
       <c r="D16">
-        <f>C16-B16</f>
+        <f t="shared" si="0"/>
         <v>-1054</v>
       </c>
     </row>
@@ -600,7 +618,7 @@
         <v>51248</v>
       </c>
       <c r="D17">
-        <f>C17-B17</f>
+        <f t="shared" si="0"/>
         <v>-1177</v>
       </c>
     </row>
@@ -615,7 +633,7 @@
         <v>53593</v>
       </c>
       <c r="D18">
-        <f>C18-B18</f>
+        <f t="shared" si="0"/>
         <v>-1194</v>
       </c>
     </row>
@@ -630,7 +648,7 @@
         <v>54001</v>
       </c>
       <c r="D19">
-        <f>C19-B19</f>
+        <f t="shared" si="0"/>
         <v>-1316</v>
       </c>
     </row>
@@ -645,8 +663,188 @@
         <v>56455</v>
       </c>
       <c r="D20">
-        <f>C20-B20</f>
+        <f t="shared" si="0"/>
         <v>-1319</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21">
+        <v>58254</v>
+      </c>
+      <c r="C21">
+        <v>56937</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>-1317</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22">
+        <v>58739</v>
+      </c>
+      <c r="C22">
+        <v>57422</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>-1317</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23">
+        <v>58912</v>
+      </c>
+      <c r="C23">
+        <v>57594</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>-1318</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24">
+        <v>59793</v>
+      </c>
+      <c r="C24">
+        <v>58475</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>-1318</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25">
+        <v>60491</v>
+      </c>
+      <c r="C25">
+        <v>59173</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>-1318</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26">
+        <v>61653</v>
+      </c>
+      <c r="C26">
+        <v>60335</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>-1318</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27">
+        <v>62340</v>
+      </c>
+      <c r="C27">
+        <v>61022</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>-1318</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28">
+        <v>63075</v>
+      </c>
+      <c r="C28">
+        <v>61757</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>-1318</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29">
+        <v>63580</v>
+      </c>
+      <c r="C29">
+        <v>62262</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>-1318</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30">
+        <v>65397</v>
+      </c>
+      <c r="C30">
+        <v>64079</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>-1318</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31">
+        <v>66367</v>
+      </c>
+      <c r="C31">
+        <v>65049</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>-1318</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32">
+        <v>67521</v>
+      </c>
+      <c r="C32">
+        <v>66203</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>-1318</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Eggerland - more levels done.
</commit_message>
<xml_diff>
--- a/trunk/Eggerland/Eggerland.xlsx
+++ b/trunk/Eggerland/Eggerland.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
   <si>
     <t>Enter room</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>Get Key</t>
+  </si>
+  <si>
+    <t>Exit Room (glitch)</t>
+  </si>
+  <si>
+    <t>Get treasure</t>
   </si>
 </sst>
 </file>
@@ -398,15 +404,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -528,7 +534,7 @@
         <v>44087</v>
       </c>
       <c r="D11">
-        <f t="shared" ref="D11:D32" si="0">C11-B11</f>
+        <f t="shared" ref="D11:D45" si="0">C11-B11</f>
         <v>-1056</v>
       </c>
     </row>
@@ -845,6 +851,201 @@
       <c r="D32">
         <f t="shared" si="0"/>
         <v>-1318</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33">
+        <v>68284</v>
+      </c>
+      <c r="C33">
+        <v>66967</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>-1317</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34">
+        <v>68894</v>
+      </c>
+      <c r="C34">
+        <v>67577</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>-1317</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35">
+        <v>70874</v>
+      </c>
+      <c r="C35">
+        <v>69557</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>-1317</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36">
+        <v>71325</v>
+      </c>
+      <c r="C36">
+        <v>70008</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>-1317</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37">
+        <v>71847</v>
+      </c>
+      <c r="C37">
+        <v>70409</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="0"/>
+        <v>-1438</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38">
+        <v>73218</v>
+      </c>
+      <c r="C38">
+        <v>71658</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>-1560</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39">
+        <v>73499</v>
+      </c>
+      <c r="C39">
+        <v>71939</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="0"/>
+        <v>-1560</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40">
+        <v>74867</v>
+      </c>
+      <c r="C40">
+        <v>73307</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="0"/>
+        <v>-1560</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41">
+        <v>75642</v>
+      </c>
+      <c r="C41">
+        <v>74082</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="0"/>
+        <v>-1560</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42">
+        <v>75931</v>
+      </c>
+      <c r="C42">
+        <v>74371</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>-1560</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43">
+        <v>76460</v>
+      </c>
+      <c r="C43">
+        <v>74779</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="0"/>
+        <v>-1681</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>18</v>
+      </c>
+      <c r="B44">
+        <v>77375</v>
+      </c>
+      <c r="C44">
+        <v>75694</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="0"/>
+        <v>-1681</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>3</v>
+      </c>
+      <c r="B45">
+        <v>77969</v>
+      </c>
+      <c r="C45">
+        <v>76165</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="0"/>
+        <v>-1804</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Eggerland - 2 more levels done.
</commit_message>
<xml_diff>
--- a/trunk/Eggerland/Eggerland.xlsx
+++ b/trunk/Eggerland/Eggerland.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
   <si>
     <t>Enter room</t>
   </si>
@@ -404,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -534,7 +534,7 @@
         <v>44087</v>
       </c>
       <c r="D11">
-        <f t="shared" ref="D11:D45" si="0">C11-B11</f>
+        <f t="shared" ref="D11:D46" si="0">C11-B11</f>
         <v>-1056</v>
       </c>
     </row>
@@ -1044,6 +1044,21 @@
         <v>76165</v>
       </c>
       <c r="D45">
+        <f t="shared" si="0"/>
+        <v>-1804</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46">
+        <v>79223</v>
+      </c>
+      <c r="C46">
+        <v>77419</v>
+      </c>
+      <c r="D46">
         <f t="shared" si="0"/>
         <v>-1804</v>
       </c>

</xml_diff>

<commit_message>
Eggerland - several more levels done.
</commit_message>
<xml_diff>
--- a/trunk/Eggerland/Eggerland.xlsx
+++ b/trunk/Eggerland/Eggerland.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="19">
   <si>
     <t>Enter room</t>
   </si>
@@ -404,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -534,7 +534,7 @@
         <v>44087</v>
       </c>
       <c r="D11">
-        <f t="shared" ref="D11:D46" si="0">C11-B11</f>
+        <f t="shared" ref="D11:D54" si="0">C11-B11</f>
         <v>-1056</v>
       </c>
     </row>
@@ -1061,6 +1061,126 @@
       <c r="D46">
         <f t="shared" si="0"/>
         <v>-1804</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>16</v>
+      </c>
+      <c r="B47">
+        <v>82883</v>
+      </c>
+      <c r="C47">
+        <v>81079</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="0"/>
+        <v>-1804</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>16</v>
+      </c>
+      <c r="B48">
+        <v>84163</v>
+      </c>
+      <c r="C48">
+        <v>82358</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="0"/>
+        <v>-1805</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>16</v>
+      </c>
+      <c r="B49">
+        <v>85727</v>
+      </c>
+      <c r="C49">
+        <v>83923</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="0"/>
+        <v>-1804</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>13</v>
+      </c>
+      <c r="B50">
+        <v>86849</v>
+      </c>
+      <c r="C50">
+        <v>85045</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="0"/>
+        <v>-1804</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51">
+        <v>87329</v>
+      </c>
+      <c r="C51">
+        <v>85525</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="0"/>
+        <v>-1804</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52">
+        <v>89980</v>
+      </c>
+      <c r="C52">
+        <v>88177</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="0"/>
+        <v>-1803</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53">
+        <v>90538</v>
+      </c>
+      <c r="C53">
+        <v>88736</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="0"/>
+        <v>-1802</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" t="s">
+        <v>4</v>
+      </c>
+      <c r="B54">
+        <v>91107</v>
+      </c>
+      <c r="C54">
+        <v>89305</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="0"/>
+        <v>-1802</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Eggerland - many more levels.  About 85% done at this point.
</commit_message>
<xml_diff>
--- a/trunk/Eggerland/Eggerland.xlsx
+++ b/trunk/Eggerland/Eggerland.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="22">
   <si>
     <t>Enter room</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t>Get treasure</t>
+  </si>
+  <si>
+    <t>Green Lolo</t>
+  </si>
+  <si>
+    <t>Level scroll</t>
+  </si>
+  <si>
+    <t>Level appear</t>
   </si>
 </sst>
 </file>
@@ -404,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:J75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -534,7 +543,7 @@
         <v>44087</v>
       </c>
       <c r="D11">
-        <f t="shared" ref="D11:D54" si="0">C11-B11</f>
+        <f t="shared" ref="D11:D75" si="0">C11-B11</f>
         <v>-1056</v>
       </c>
     </row>
@@ -1093,7 +1102,7 @@
         <v>-1805</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:10">
       <c r="A49" t="s">
         <v>16</v>
       </c>
@@ -1108,7 +1117,7 @@
         <v>-1804</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:10">
       <c r="A50" t="s">
         <v>13</v>
       </c>
@@ -1123,7 +1132,7 @@
         <v>-1804</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:10">
       <c r="A51" t="s">
         <v>5</v>
       </c>
@@ -1138,7 +1147,7 @@
         <v>-1804</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:10">
       <c r="A52" t="s">
         <v>12</v>
       </c>
@@ -1153,7 +1162,7 @@
         <v>-1803</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:10">
       <c r="A53" t="s">
         <v>5</v>
       </c>
@@ -1168,7 +1177,7 @@
         <v>-1802</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:10">
       <c r="A54" t="s">
         <v>4</v>
       </c>
@@ -1181,6 +1190,334 @@
       <c r="D54">
         <f t="shared" si="0"/>
         <v>-1802</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55">
+        <v>92262</v>
+      </c>
+      <c r="C55">
+        <v>90460</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="0"/>
+        <v>-1802</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56" t="s">
+        <v>19</v>
+      </c>
+      <c r="B56">
+        <v>92927</v>
+      </c>
+      <c r="C56">
+        <v>91126</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="0"/>
+        <v>-1801</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="A57" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57">
+        <v>93439</v>
+      </c>
+      <c r="C57">
+        <v>91638</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="0"/>
+        <v>-1801</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="A58" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58">
+        <v>96846</v>
+      </c>
+      <c r="C58">
+        <v>95046</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="0"/>
+        <v>-1800</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="A59" t="s">
+        <v>8</v>
+      </c>
+      <c r="B59">
+        <v>97744</v>
+      </c>
+      <c r="C59">
+        <v>95821</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="0"/>
+        <v>-1923</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="B60">
+        <v>98315</v>
+      </c>
+      <c r="C60">
+        <v>96392</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="0"/>
+        <v>-1923</v>
+      </c>
+      <c r="J60">
+        <f>5/6</f>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="A61" t="s">
+        <v>18</v>
+      </c>
+      <c r="B61">
+        <v>98587</v>
+      </c>
+      <c r="C61">
+        <v>96664</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="0"/>
+        <v>-1923</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="A62" t="s">
+        <v>8</v>
+      </c>
+      <c r="B62">
+        <v>99181</v>
+      </c>
+      <c r="C62">
+        <v>97136</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="0"/>
+        <v>-2045</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="A63" t="s">
+        <v>8</v>
+      </c>
+      <c r="B63">
+        <v>99784</v>
+      </c>
+      <c r="C63">
+        <v>97739</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="0"/>
+        <v>-2045</v>
+      </c>
+      <c r="I63">
+        <f>123*3</f>
+        <v>369</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="A64" t="s">
+        <v>20</v>
+      </c>
+      <c r="B64">
+        <v>102281</v>
+      </c>
+      <c r="C64">
+        <v>100238</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="0"/>
+        <v>-2043</v>
+      </c>
+      <c r="I64">
+        <f>369+2298</f>
+        <v>2667</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" t="s">
+        <v>20</v>
+      </c>
+      <c r="B65">
+        <v>102435</v>
+      </c>
+      <c r="C65">
+        <v>100392</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="0"/>
+        <v>-2043</v>
+      </c>
+      <c r="I65">
+        <f>I64/60</f>
+        <v>44.45</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66" t="s">
+        <v>5</v>
+      </c>
+      <c r="B66">
+        <v>104783</v>
+      </c>
+      <c r="C66">
+        <v>102732</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="0"/>
+        <v>-2051</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" t="s">
+        <v>5</v>
+      </c>
+      <c r="B67">
+        <v>105147</v>
+      </c>
+      <c r="C67">
+        <v>103096</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="0"/>
+        <v>-2051</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68" t="s">
+        <v>21</v>
+      </c>
+      <c r="B68">
+        <v>105798</v>
+      </c>
+      <c r="C68">
+        <v>103624</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="0"/>
+        <v>-2174</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="A69" t="s">
+        <v>18</v>
+      </c>
+      <c r="B69">
+        <v>106665</v>
+      </c>
+      <c r="C69">
+        <v>104491</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="0"/>
+        <v>-2174</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70" t="s">
+        <v>21</v>
+      </c>
+      <c r="B70">
+        <v>107257</v>
+      </c>
+      <c r="C70">
+        <v>104959</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="0"/>
+        <v>-2298</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71" t="s">
+        <v>5</v>
+      </c>
+      <c r="B71">
+        <v>110558</v>
+      </c>
+      <c r="C71">
+        <v>108260</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="0"/>
+        <v>-2298</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72" t="s">
+        <v>5</v>
+      </c>
+      <c r="B72">
+        <v>112188</v>
+      </c>
+      <c r="C72">
+        <v>109890</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="0"/>
+        <v>-2298</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="A73" t="s">
+        <v>5</v>
+      </c>
+      <c r="B73">
+        <v>113158</v>
+      </c>
+      <c r="C73">
+        <v>110860</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="0"/>
+        <v>-2298</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="A74" t="s">
+        <v>5</v>
+      </c>
+      <c r="B74">
+        <v>115248</v>
+      </c>
+      <c r="C74">
+        <v>112951</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="0"/>
+        <v>-2297</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="A75" t="s">
+        <v>5</v>
+      </c>
+      <c r="B75">
+        <v>116008</v>
+      </c>
+      <c r="C75">
+        <v>113711</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="0"/>
+        <v>-2297</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Eggerland - movie done!
</commit_message>
<xml_diff>
--- a/trunk/Eggerland/Eggerland.xlsx
+++ b/trunk/Eggerland/Eggerland.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="23">
   <si>
     <t>Enter room</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Level appear</t>
+  </si>
+  <si>
+    <t>Key appears</t>
   </si>
 </sst>
 </file>
@@ -413,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -543,7 +546,7 @@
         <v>44087</v>
       </c>
       <c r="D11">
-        <f t="shared" ref="D11:D75" si="0">C11-B11</f>
+        <f t="shared" ref="D11:D91" si="0">C11-B11</f>
         <v>-1056</v>
       </c>
     </row>
@@ -1518,6 +1521,243 @@
       <c r="D75">
         <f t="shared" si="0"/>
         <v>-2297</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="A76" t="s">
+        <v>22</v>
+      </c>
+      <c r="B76">
+        <v>120939</v>
+      </c>
+      <c r="C76">
+        <v>118643</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="0"/>
+        <v>-2296</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="A77" t="s">
+        <v>5</v>
+      </c>
+      <c r="B77">
+        <v>121084</v>
+      </c>
+      <c r="C77">
+        <v>118788</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="0"/>
+        <v>-2296</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
+      <c r="A78" t="s">
+        <v>3</v>
+      </c>
+      <c r="B78">
+        <v>121665</v>
+      </c>
+      <c r="C78">
+        <v>119246</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="0"/>
+        <v>-2419</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9">
+      <c r="A79" t="s">
+        <v>18</v>
+      </c>
+      <c r="B79">
+        <v>122084</v>
+      </c>
+      <c r="C79">
+        <v>119665</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="0"/>
+        <v>-2419</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9">
+      <c r="A80" t="s">
+        <v>3</v>
+      </c>
+      <c r="B80">
+        <v>122678</v>
+      </c>
+      <c r="C80">
+        <v>120135</v>
+      </c>
+      <c r="D80">
+        <f t="shared" si="0"/>
+        <v>-2543</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" t="s">
+        <v>9</v>
+      </c>
+      <c r="B81">
+        <v>124219</v>
+      </c>
+      <c r="C81">
+        <v>121676</v>
+      </c>
+      <c r="D81">
+        <f t="shared" si="0"/>
+        <v>-2543</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" t="s">
+        <v>3</v>
+      </c>
+      <c r="B82">
+        <v>124750</v>
+      </c>
+      <c r="C82">
+        <v>122084</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="0"/>
+        <v>-2666</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" t="s">
+        <v>3</v>
+      </c>
+      <c r="B83">
+        <v>125026</v>
+      </c>
+      <c r="C83">
+        <v>122360</v>
+      </c>
+      <c r="D83">
+        <f t="shared" si="0"/>
+        <v>-2666</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" t="s">
+        <v>16</v>
+      </c>
+      <c r="B84">
+        <v>126650</v>
+      </c>
+      <c r="C84">
+        <v>123985</v>
+      </c>
+      <c r="D84">
+        <f t="shared" si="0"/>
+        <v>-2665</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" t="s">
+        <v>4</v>
+      </c>
+      <c r="C85">
+        <v>125324</v>
+      </c>
+      <c r="D85">
+        <f t="shared" si="0"/>
+        <v>125324</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" t="s">
+        <v>5</v>
+      </c>
+      <c r="B86">
+        <v>129103</v>
+      </c>
+      <c r="C86">
+        <v>126438</v>
+      </c>
+      <c r="D86">
+        <f t="shared" si="0"/>
+        <v>-2665</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" t="s">
+        <v>4</v>
+      </c>
+      <c r="B87">
+        <v>129917</v>
+      </c>
+      <c r="C87">
+        <v>127252</v>
+      </c>
+      <c r="D87">
+        <f t="shared" si="0"/>
+        <v>-2665</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" t="s">
+        <v>5</v>
+      </c>
+      <c r="B88">
+        <v>130061</v>
+      </c>
+      <c r="C88">
+        <v>127396</v>
+      </c>
+      <c r="D88">
+        <f t="shared" si="0"/>
+        <v>-2665</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" t="s">
+        <v>5</v>
+      </c>
+      <c r="B89">
+        <v>130939</v>
+      </c>
+      <c r="C89">
+        <v>128274</v>
+      </c>
+      <c r="D89">
+        <f t="shared" si="0"/>
+        <v>-2665</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" t="s">
+        <v>5</v>
+      </c>
+      <c r="B90">
+        <v>131427</v>
+      </c>
+      <c r="C90">
+        <v>128763</v>
+      </c>
+      <c r="D90">
+        <f t="shared" si="0"/>
+        <v>-2664</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" t="s">
+        <v>5</v>
+      </c>
+      <c r="B91">
+        <v>133230</v>
+      </c>
+      <c r="C91">
+        <v>130565</v>
+      </c>
+      <c r="D91">
+        <f t="shared" si="0"/>
+        <v>-2665</v>
       </c>
     </row>
   </sheetData>

</xml_diff>